<commit_message>
add Michael Kane to attendee spreadsheet
</commit_message>
<xml_diff>
--- a/data/wg_attendees.xlsx
+++ b/data/wg_attendees.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="248" uniqueCount="149">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="251" uniqueCount="152">
   <si>
     <t xml:space="preserve">name</t>
   </si>
@@ -466,25 +466,16 @@
     <t xml:space="preserve">Boehringer Ingelheim</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF0000FF"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">https://www.boehringer-ingelheim.com/</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
+    <t xml:space="preserve">https://www.boehringer-ingelheim.com/ </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Michael Kane</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MD Anderson Cancer Institute</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://www.mdanderson.org/ </t>
   </si>
 </sst>
 </file>
@@ -596,21 +587,21 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C83"/>
+  <dimension ref="A1:C84"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A34" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C84" activeCellId="0" sqref="C84"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A70" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B85" activeCellId="0" sqref="B85"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="28.09"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="28.11"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="37.41"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="36.3"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="36.31"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1521,6 +1512,17 @@
       </c>
       <c r="C83" s="2" t="s">
         <v>148</v>
+      </c>
+    </row>
+    <row r="84" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A84" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="B84" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="C84" s="2" t="s">
+        <v>151</v>
       </c>
     </row>
   </sheetData>
@@ -1605,7 +1607,8 @@
     <hyperlink ref="C80" r:id="rId78" display="https://www.gene.com"/>
     <hyperlink ref="C81" r:id="rId79" display="https://www.regeneron.com "/>
     <hyperlink ref="C82" r:id="rId80" display="https://www.gsk.com/en-gb/home/ "/>
-    <hyperlink ref="C83" r:id="rId81" display="https://www.boehringer-ingelheim.com/"/>
+    <hyperlink ref="C83" r:id="rId81" display="https://www.boehringer-ingelheim.com/ "/>
+    <hyperlink ref="C84" r:id="rId82" display="https://www.mdanderson.org/ "/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>

<commit_message>
Minutes for 10-04-2024 and new dev setup (#126)
* revise devcontainer setup

* fix space issue in minutes template block

* update attendee spreadsheet

* add minutes for 10-04-2024 WG meeting
</commit_message>
<xml_diff>
--- a/data/wg_attendees.xlsx
+++ b/data/wg_attendees.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="251" uniqueCount="152">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="266" uniqueCount="159">
   <si>
     <t xml:space="preserve">name</t>
   </si>
@@ -476,6 +476,45 @@
   </si>
   <si>
     <t xml:space="preserve">https://www.mdanderson.org/ </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Terry Christiani</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Amanda Martin</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Andre Couturier</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sanofi</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF0000FF"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">https://www.sanofi.com/</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">Nicholas Masel</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Lovemore Gakava</t>
   </si>
 </sst>
 </file>
@@ -587,21 +626,21 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C84"/>
+  <dimension ref="A1:C89"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A70" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B85" activeCellId="0" sqref="B85"/>
+      <selection pane="topLeft" activeCell="A70" activeCellId="0" sqref="A70"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="28.11"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="37.41"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="36.31"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="36.3"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1523,6 +1562,61 @@
       </c>
       <c r="C84" s="2" t="s">
         <v>151</v>
+      </c>
+    </row>
+    <row r="85" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A85" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="B85" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C85" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="86" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A86" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="B86" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C86" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="87" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A87" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="B87" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="C87" s="2" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="88" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A88" s="1" t="s">
+        <v>157</v>
+      </c>
+      <c r="B88" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="C88" s="2" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="89" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A89" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="B89" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="C89" s="2" t="s">
+        <v>86</v>
       </c>
     </row>
   </sheetData>
@@ -1609,6 +1703,11 @@
     <hyperlink ref="C82" r:id="rId80" display="https://www.gsk.com/en-gb/home/ "/>
     <hyperlink ref="C83" r:id="rId81" display="https://www.boehringer-ingelheim.com/ "/>
     <hyperlink ref="C84" r:id="rId82" display="https://www.mdanderson.org/ "/>
+    <hyperlink ref="C85" r:id="rId83" display="https://www.r-consortium.org"/>
+    <hyperlink ref="C86" r:id="rId84" display="https://www.r-consortium.org"/>
+    <hyperlink ref="C87" r:id="rId85" display="https://www.sanofi.com/"/>
+    <hyperlink ref="C88" r:id="rId86" display="https://www.jnj.com"/>
+    <hyperlink ref="C89" r:id="rId87" display="https://www.novonordisk.com/ "/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>

<commit_message>
add new attendees Katie Harding and Youn Kyeong Chang
</commit_message>
<xml_diff>
--- a/data/wg_attendees.xlsx
+++ b/data/wg_attendees.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="266" uniqueCount="159">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="272" uniqueCount="163">
   <si>
     <t xml:space="preserve">name</t>
   </si>
@@ -488,6 +488,21 @@
   </si>
   <si>
     <t xml:space="preserve">Sanofi</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://www.sanofi.com/ </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nicholas Masel</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Lovemore Gakava</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Katie Harding</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Freenome</t>
   </si>
   <si>
     <r>
@@ -498,7 +513,7 @@
         <family val="2"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve">https://www.sanofi.com/</t>
+      <t xml:space="preserve">https://www.freenome.com/</t>
     </r>
     <r>
       <rPr>
@@ -511,10 +526,7 @@
     </r>
   </si>
   <si>
-    <t xml:space="preserve">Nicholas Masel</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Lovemore Gakava</t>
+    <t xml:space="preserve">Youn Kyeong Chang</t>
   </si>
 </sst>
 </file>
@@ -626,21 +638,21 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C89"/>
+  <dimension ref="A1:C91"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A70" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A70" activeCellId="0" sqref="A70"/>
+      <selection pane="topLeft" activeCell="C91" activeCellId="0" sqref="C91"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="28.11"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="37.41"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="36.3"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="36.31"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1617,6 +1629,28 @@
       </c>
       <c r="C89" s="2" t="s">
         <v>86</v>
+      </c>
+    </row>
+    <row r="90" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A90" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="B90" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="C90" s="2" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="91" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A91" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="B91" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C91" s="2" t="s">
+        <v>32</v>
       </c>
     </row>
   </sheetData>
@@ -1705,9 +1739,11 @@
     <hyperlink ref="C84" r:id="rId82" display="https://www.mdanderson.org/ "/>
     <hyperlink ref="C85" r:id="rId83" display="https://www.r-consortium.org"/>
     <hyperlink ref="C86" r:id="rId84" display="https://www.r-consortium.org"/>
-    <hyperlink ref="C87" r:id="rId85" display="https://www.sanofi.com/"/>
+    <hyperlink ref="C87" r:id="rId85" display="https://www.sanofi.com/ "/>
     <hyperlink ref="C88" r:id="rId86" display="https://www.jnj.com"/>
     <hyperlink ref="C89" r:id="rId87" display="https://www.novonordisk.com/ "/>
+    <hyperlink ref="C90" r:id="rId88" display="https://www.freenome.com/"/>
+    <hyperlink ref="C91" r:id="rId89" display="https://www.fda.gov/"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>

<commit_message>
Minutes for 2024-11-01 working group meeting (#128)
* add new attendees Katie Harding and Youn Kyeong Chang

* open external links in a new tab

* add minutes for 2024-11-01 working group meeting

* update default date for minutes gen page
</commit_message>
<xml_diff>
--- a/data/wg_attendees.xlsx
+++ b/data/wg_attendees.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="266" uniqueCount="159">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="272" uniqueCount="163">
   <si>
     <t xml:space="preserve">name</t>
   </si>
@@ -488,6 +488,21 @@
   </si>
   <si>
     <t xml:space="preserve">Sanofi</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://www.sanofi.com/ </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nicholas Masel</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Lovemore Gakava</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Katie Harding</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Freenome</t>
   </si>
   <si>
     <r>
@@ -498,7 +513,7 @@
         <family val="2"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve">https://www.sanofi.com/</t>
+      <t xml:space="preserve">https://www.freenome.com/</t>
     </r>
     <r>
       <rPr>
@@ -511,10 +526,7 @@
     </r>
   </si>
   <si>
-    <t xml:space="preserve">Nicholas Masel</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Lovemore Gakava</t>
+    <t xml:space="preserve">Youn Kyeong Chang</t>
   </si>
 </sst>
 </file>
@@ -626,21 +638,21 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C89"/>
+  <dimension ref="A1:C91"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A70" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A70" activeCellId="0" sqref="A70"/>
+      <selection pane="topLeft" activeCell="C91" activeCellId="0" sqref="C91"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="28.11"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="37.41"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="36.3"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="36.31"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1617,6 +1629,28 @@
       </c>
       <c r="C89" s="2" t="s">
         <v>86</v>
+      </c>
+    </row>
+    <row r="90" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A90" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="B90" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="C90" s="2" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="91" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A91" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="B91" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C91" s="2" t="s">
+        <v>32</v>
       </c>
     </row>
   </sheetData>
@@ -1705,9 +1739,11 @@
     <hyperlink ref="C84" r:id="rId82" display="https://www.mdanderson.org/ "/>
     <hyperlink ref="C85" r:id="rId83" display="https://www.r-consortium.org"/>
     <hyperlink ref="C86" r:id="rId84" display="https://www.r-consortium.org"/>
-    <hyperlink ref="C87" r:id="rId85" display="https://www.sanofi.com/"/>
+    <hyperlink ref="C87" r:id="rId85" display="https://www.sanofi.com/ "/>
     <hyperlink ref="C88" r:id="rId86" display="https://www.jnj.com"/>
     <hyperlink ref="C89" r:id="rId87" display="https://www.novonordisk.com/ "/>
+    <hyperlink ref="C90" r:id="rId88" display="https://www.freenome.com/"/>
+    <hyperlink ref="C91" r:id="rId89" display="https://www.fda.gov/"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>

<commit_message>
fix: add Sam Hume to attendees spreadsheet
</commit_message>
<xml_diff>
--- a/data/wg_attendees.xlsx
+++ b/data/wg_attendees.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="272" uniqueCount="163">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="275" uniqueCount="166">
   <si>
     <t xml:space="preserve">name</t>
   </si>
@@ -503,6 +503,18 @@
   </si>
   <si>
     <t xml:space="preserve">Freenome</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://www.freenome.com/ </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Youn Kyeong Chang</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sam Hume</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CDISC</t>
   </si>
   <si>
     <r>
@@ -513,7 +525,7 @@
         <family val="2"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve">https://www.freenome.com/</t>
+      <t xml:space="preserve">https://www.cdisc.org/</t>
     </r>
     <r>
       <rPr>
@@ -524,9 +536,6 @@
       </rPr>
       <t xml:space="preserve"> </t>
     </r>
-  </si>
-  <si>
-    <t xml:space="preserve">Youn Kyeong Chang</t>
   </si>
 </sst>
 </file>
@@ -642,13 +651,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C91"/>
+  <dimension ref="A1:C92"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A70" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C91" activeCellId="0" sqref="C91"/>
+      <selection pane="topLeft" activeCell="A93" activeCellId="0" sqref="A93"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="28.11"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="37.41"/>
@@ -1651,6 +1660,17 @@
       </c>
       <c r="C91" s="2" t="s">
         <v>32</v>
+      </c>
+    </row>
+    <row r="92" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A92" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="B92" s="1" t="s">
+        <v>164</v>
+      </c>
+      <c r="C92" s="2" t="s">
+        <v>165</v>
       </c>
     </row>
   </sheetData>
@@ -1742,8 +1762,9 @@
     <hyperlink ref="C87" r:id="rId85" display="https://www.sanofi.com/ "/>
     <hyperlink ref="C88" r:id="rId86" display="https://www.jnj.com"/>
     <hyperlink ref="C89" r:id="rId87" display="https://www.novonordisk.com/ "/>
-    <hyperlink ref="C90" r:id="rId88" display="https://www.freenome.com/"/>
+    <hyperlink ref="C90" r:id="rId88" display="https://www.freenome.com/ "/>
     <hyperlink ref="C91" r:id="rId89" display="https://www.fda.gov/"/>
+    <hyperlink ref="C92" r:id="rId90" display="https://www.cdisc.org/"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>

<commit_message>
Add minutes for 12-06-2024 meeting (#132)
* docs: add 12-06-2024 minutes
* fix: add Sam Hume to attendees spreadsheet
* feat: enable GH action for site preview
</commit_message>
<xml_diff>
--- a/data/wg_attendees.xlsx
+++ b/data/wg_attendees.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="272" uniqueCount="163">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="275" uniqueCount="166">
   <si>
     <t xml:space="preserve">name</t>
   </si>
@@ -503,6 +503,18 @@
   </si>
   <si>
     <t xml:space="preserve">Freenome</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://www.freenome.com/ </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Youn Kyeong Chang</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sam Hume</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CDISC</t>
   </si>
   <si>
     <r>
@@ -513,7 +525,7 @@
         <family val="2"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve">https://www.freenome.com/</t>
+      <t xml:space="preserve">https://www.cdisc.org/</t>
     </r>
     <r>
       <rPr>
@@ -524,9 +536,6 @@
       </rPr>
       <t xml:space="preserve"> </t>
     </r>
-  </si>
-  <si>
-    <t xml:space="preserve">Youn Kyeong Chang</t>
   </si>
 </sst>
 </file>
@@ -642,13 +651,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C91"/>
+  <dimension ref="A1:C92"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A70" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C91" activeCellId="0" sqref="C91"/>
+      <selection pane="topLeft" activeCell="A93" activeCellId="0" sqref="A93"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="28.11"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="37.41"/>
@@ -1651,6 +1660,17 @@
       </c>
       <c r="C91" s="2" t="s">
         <v>32</v>
+      </c>
+    </row>
+    <row r="92" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A92" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="B92" s="1" t="s">
+        <v>164</v>
+      </c>
+      <c r="C92" s="2" t="s">
+        <v>165</v>
       </c>
     </row>
   </sheetData>
@@ -1742,8 +1762,9 @@
     <hyperlink ref="C87" r:id="rId85" display="https://www.sanofi.com/ "/>
     <hyperlink ref="C88" r:id="rId86" display="https://www.jnj.com"/>
     <hyperlink ref="C89" r:id="rId87" display="https://www.novonordisk.com/ "/>
-    <hyperlink ref="C90" r:id="rId88" display="https://www.freenome.com/"/>
+    <hyperlink ref="C90" r:id="rId88" display="https://www.freenome.com/ "/>
     <hyperlink ref="C91" r:id="rId89" display="https://www.fda.gov/"/>
+    <hyperlink ref="C92" r:id="rId90" display="https://www.cdisc.org/"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>

<commit_message>
fix: update attendees spreadsheet
</commit_message>
<xml_diff>
--- a/data/wg_attendees.xlsx
+++ b/data/wg_attendees.xlsx
@@ -8,7 +8,7 @@
     <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId3"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="275" uniqueCount="166">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="283" uniqueCount="174">
   <si>
     <t xml:space="preserve">name</t>
   </si>
@@ -517,25 +517,31 @@
     <t xml:space="preserve">CDISC</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF0000FF"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">https://www.cdisc.org/</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
+    <t xml:space="preserve">https://www.cdisc.org/ </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Camille Calmasini</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Natera</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://www.natera.com/</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Jim Rothstein</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Freelance</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nabil Baugher</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Baseline AI</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://www.baselinetrials.com</t>
   </si>
 </sst>
 </file>
@@ -545,7 +551,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="6">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -566,6 +572,13 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF0000FF"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -617,7 +630,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -634,6 +647,10 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -646,22 +663,128 @@
 </styleSheet>
 </file>
 
+<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Office">
+  <a:themeElements>
+    <a:clrScheme name="LibreOffice">
+      <a:dk1>
+        <a:srgbClr val="000000"/>
+      </a:dk1>
+      <a:lt1>
+        <a:srgbClr val="ffffff"/>
+      </a:lt1>
+      <a:dk2>
+        <a:srgbClr val="000000"/>
+      </a:dk2>
+      <a:lt2>
+        <a:srgbClr val="ffffff"/>
+      </a:lt2>
+      <a:accent1>
+        <a:srgbClr val="18a303"/>
+      </a:accent1>
+      <a:accent2>
+        <a:srgbClr val="0369a3"/>
+      </a:accent2>
+      <a:accent3>
+        <a:srgbClr val="a33e03"/>
+      </a:accent3>
+      <a:accent4>
+        <a:srgbClr val="8e03a3"/>
+      </a:accent4>
+      <a:accent5>
+        <a:srgbClr val="c99c00"/>
+      </a:accent5>
+      <a:accent6>
+        <a:srgbClr val="c9211e"/>
+      </a:accent6>
+      <a:hlink>
+        <a:srgbClr val="0000ee"/>
+      </a:hlink>
+      <a:folHlink>
+        <a:srgbClr val="551a8b"/>
+      </a:folHlink>
+    </a:clrScheme>
+    <a:fontScheme name="Office">
+      <a:majorFont>
+        <a:latin typeface="Arial" pitchFamily="0" charset="1"/>
+        <a:ea typeface="DejaVu Sans" pitchFamily="0" charset="1"/>
+        <a:cs typeface="DejaVu Sans" pitchFamily="0" charset="1"/>
+      </a:majorFont>
+      <a:minorFont>
+        <a:latin typeface="Arial" pitchFamily="0" charset="1"/>
+        <a:ea typeface="DejaVu Sans" pitchFamily="0" charset="1"/>
+        <a:cs typeface="DejaVu Sans" pitchFamily="0" charset="1"/>
+      </a:minorFont>
+    </a:fontScheme>
+    <a:fmtScheme>
+      <a:fillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:fillStyleLst>
+      <a:lnStyleLst>
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+          <a:prstDash val="solid"/>
+          <a:miter/>
+        </a:ln>
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+          <a:prstDash val="solid"/>
+          <a:miter/>
+        </a:ln>
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+          <a:prstDash val="solid"/>
+          <a:miter/>
+        </a:ln>
+      </a:lnStyleLst>
+      <a:effectStyleLst>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+      </a:effectStyleLst>
+      <a:bgFillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:bgFillStyleLst>
+    </a:fmtScheme>
+  </a:themeElements>
+</a:theme>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C92"/>
+  <dimension ref="A1:C95"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A70" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A93" activeCellId="0" sqref="A93"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A55" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A96" activeCellId="0" sqref="A96"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="28.11"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="37.41"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="36.31"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="36.3"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1671,6 +1794,36 @@
       </c>
       <c r="C92" s="2" t="s">
         <v>165</v>
+      </c>
+    </row>
+    <row r="93" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A93" s="1" t="s">
+        <v>166</v>
+      </c>
+      <c r="B93" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="C93" s="4" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="94" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A94" s="1" t="s">
+        <v>169</v>
+      </c>
+      <c r="B94" s="1" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="95" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A95" s="1" t="s">
+        <v>171</v>
+      </c>
+      <c r="B95" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="C95" s="4" t="s">
+        <v>173</v>
       </c>
     </row>
   </sheetData>
@@ -1764,7 +1917,9 @@
     <hyperlink ref="C89" r:id="rId87" display="https://www.novonordisk.com/ "/>
     <hyperlink ref="C90" r:id="rId88" display="https://www.freenome.com/ "/>
     <hyperlink ref="C91" r:id="rId89" display="https://www.fda.gov/"/>
-    <hyperlink ref="C92" r:id="rId90" display="https://www.cdisc.org/"/>
+    <hyperlink ref="C92" r:id="rId90" display="https://www.cdisc.org/ "/>
+    <hyperlink ref="C93" r:id="rId91" display="https://www.natera.com/"/>
+    <hyperlink ref="C95" r:id="rId92" display="https://www.baselinetrials.com"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>

<commit_message>
feat: add minutes for 4-4-2025 WG meeting (#142)
</commit_message>
<xml_diff>
--- a/data/wg_attendees.xlsx
+++ b/data/wg_attendees.xlsx
@@ -8,7 +8,7 @@
     <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId3"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="275" uniqueCount="166">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="283" uniqueCount="174">
   <si>
     <t xml:space="preserve">name</t>
   </si>
@@ -517,25 +517,31 @@
     <t xml:space="preserve">CDISC</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF0000FF"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">https://www.cdisc.org/</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
+    <t xml:space="preserve">https://www.cdisc.org/ </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Camille Calmasini</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Natera</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://www.natera.com/</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Jim Rothstein</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Freelance</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nabil Baugher</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Baseline AI</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://www.baselinetrials.com</t>
   </si>
 </sst>
 </file>
@@ -545,7 +551,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="6">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -566,6 +572,13 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF0000FF"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -617,7 +630,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -634,6 +647,10 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -646,22 +663,128 @@
 </styleSheet>
 </file>
 
+<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Office">
+  <a:themeElements>
+    <a:clrScheme name="LibreOffice">
+      <a:dk1>
+        <a:srgbClr val="000000"/>
+      </a:dk1>
+      <a:lt1>
+        <a:srgbClr val="ffffff"/>
+      </a:lt1>
+      <a:dk2>
+        <a:srgbClr val="000000"/>
+      </a:dk2>
+      <a:lt2>
+        <a:srgbClr val="ffffff"/>
+      </a:lt2>
+      <a:accent1>
+        <a:srgbClr val="18a303"/>
+      </a:accent1>
+      <a:accent2>
+        <a:srgbClr val="0369a3"/>
+      </a:accent2>
+      <a:accent3>
+        <a:srgbClr val="a33e03"/>
+      </a:accent3>
+      <a:accent4>
+        <a:srgbClr val="8e03a3"/>
+      </a:accent4>
+      <a:accent5>
+        <a:srgbClr val="c99c00"/>
+      </a:accent5>
+      <a:accent6>
+        <a:srgbClr val="c9211e"/>
+      </a:accent6>
+      <a:hlink>
+        <a:srgbClr val="0000ee"/>
+      </a:hlink>
+      <a:folHlink>
+        <a:srgbClr val="551a8b"/>
+      </a:folHlink>
+    </a:clrScheme>
+    <a:fontScheme name="Office">
+      <a:majorFont>
+        <a:latin typeface="Arial" pitchFamily="0" charset="1"/>
+        <a:ea typeface="DejaVu Sans" pitchFamily="0" charset="1"/>
+        <a:cs typeface="DejaVu Sans" pitchFamily="0" charset="1"/>
+      </a:majorFont>
+      <a:minorFont>
+        <a:latin typeface="Arial" pitchFamily="0" charset="1"/>
+        <a:ea typeface="DejaVu Sans" pitchFamily="0" charset="1"/>
+        <a:cs typeface="DejaVu Sans" pitchFamily="0" charset="1"/>
+      </a:minorFont>
+    </a:fontScheme>
+    <a:fmtScheme>
+      <a:fillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:fillStyleLst>
+      <a:lnStyleLst>
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+          <a:prstDash val="solid"/>
+          <a:miter/>
+        </a:ln>
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+          <a:prstDash val="solid"/>
+          <a:miter/>
+        </a:ln>
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+          <a:prstDash val="solid"/>
+          <a:miter/>
+        </a:ln>
+      </a:lnStyleLst>
+      <a:effectStyleLst>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+      </a:effectStyleLst>
+      <a:bgFillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:bgFillStyleLst>
+    </a:fmtScheme>
+  </a:themeElements>
+</a:theme>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C92"/>
+  <dimension ref="A1:C95"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A70" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A93" activeCellId="0" sqref="A93"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A55" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A96" activeCellId="0" sqref="A96"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="28.11"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="37.41"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="36.31"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="36.3"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1671,6 +1794,36 @@
       </c>
       <c r="C92" s="2" t="s">
         <v>165</v>
+      </c>
+    </row>
+    <row r="93" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A93" s="1" t="s">
+        <v>166</v>
+      </c>
+      <c r="B93" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="C93" s="4" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="94" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A94" s="1" t="s">
+        <v>169</v>
+      </c>
+      <c r="B94" s="1" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="95" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A95" s="1" t="s">
+        <v>171</v>
+      </c>
+      <c r="B95" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="C95" s="4" t="s">
+        <v>173</v>
       </c>
     </row>
   </sheetData>
@@ -1764,7 +1917,9 @@
     <hyperlink ref="C89" r:id="rId87" display="https://www.novonordisk.com/ "/>
     <hyperlink ref="C90" r:id="rId88" display="https://www.freenome.com/ "/>
     <hyperlink ref="C91" r:id="rId89" display="https://www.fda.gov/"/>
-    <hyperlink ref="C92" r:id="rId90" display="https://www.cdisc.org/"/>
+    <hyperlink ref="C92" r:id="rId90" display="https://www.cdisc.org/ "/>
+    <hyperlink ref="C93" r:id="rId91" display="https://www.natera.com/"/>
+    <hyperlink ref="C95" r:id="rId92" display="https://www.baselinetrials.com"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>